<commit_message>
Aetna 20 Test cases Done
</commit_message>
<xml_diff>
--- a/aetna/src/main/resources/Aetna_Employerspage_Elements.xlsx
+++ b/aetna/src/main/resources/Aetna_Employerspage_Elements.xlsx
@@ -8,12 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\IdeaProjects\AutomationFramework_Team3\aetna\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04EA4317-2D2D-4475-A507-F3E5CCC1DB84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E448A7-941D-4123-9AE1-52E8F10B80A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1065" yWindow="3675" windowWidth="2400" windowHeight="585" xr2:uid="{E4158527-C88E-47FC-8012-7E19A3D633D3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="909" firstSheet="6" activeTab="13" xr2:uid="{E4158527-C88E-47FC-8012-7E19A3D633D3}"/>
   </bookViews>
   <sheets>
     <sheet name="EmployersPageURL" sheetId="1" r:id="rId1"/>
+    <sheet name="ProductsAndServicesDropDown" sheetId="2" r:id="rId2"/>
+    <sheet name="Healthplans" sheetId="3" r:id="rId3"/>
+    <sheet name="MemberPrograms" sheetId="4" r:id="rId4"/>
+    <sheet name="AdministrationOfferings" sheetId="5" r:id="rId5"/>
+    <sheet name="ByCompanySize" sheetId="8" r:id="rId6"/>
+    <sheet name="ByIndustry" sheetId="9" r:id="rId7"/>
+    <sheet name="Solutions1" sheetId="6" r:id="rId8"/>
+    <sheet name="Solutions2" sheetId="7" r:id="rId9"/>
+    <sheet name="Resources1" sheetId="10" r:id="rId10"/>
+    <sheet name="Resources2" sheetId="13" r:id="rId11"/>
+    <sheet name="ToolsManualsForms" sheetId="12" r:id="rId12"/>
+    <sheet name="PayYourBill" sheetId="11" r:id="rId13"/>
+    <sheet name="TrendsAndInsights" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,9 +44,153 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>https://www.aetna.com/employers-organizations.html</t>
+  </si>
+  <si>
+    <t>Health plans</t>
+  </si>
+  <si>
+    <t>Member programs</t>
+  </si>
+  <si>
+    <t>Administration offerings</t>
+  </si>
+  <si>
+    <t>All health plans</t>
+  </si>
+  <si>
+    <t>Medicare</t>
+  </si>
+  <si>
+    <t>Dental</t>
+  </si>
+  <si>
+    <t>Vision</t>
+  </si>
+  <si>
+    <t>Pharmacy</t>
+  </si>
+  <si>
+    <t>Supplemental</t>
+  </si>
+  <si>
+    <t>All member programs</t>
+  </si>
+  <si>
+    <t>Aetna Health app</t>
+  </si>
+  <si>
+    <t>Behavioral health</t>
+  </si>
+  <si>
+    <t>Care management</t>
+  </si>
+  <si>
+    <t>Customer service</t>
+  </si>
+  <si>
+    <t>Diabetes</t>
+  </si>
+  <si>
+    <t>Member Engagement Platform</t>
+  </si>
+  <si>
+    <t>Telehealth</t>
+  </si>
+  <si>
+    <t>Women's health</t>
+  </si>
+  <si>
+    <t>All administration tools</t>
+  </si>
+  <si>
+    <t>PayFlex</t>
+  </si>
+  <si>
+    <t>By company size</t>
+  </si>
+  <si>
+    <t>By industry</t>
+  </si>
+  <si>
+    <t>Wellness programs</t>
+  </si>
+  <si>
+    <t>Get a quote</t>
+  </si>
+  <si>
+    <t>Small business (100 or less employees)</t>
+  </si>
+  <si>
+    <t>Mid-size business (101-4,999 employees)</t>
+  </si>
+  <si>
+    <t>Large business (5,000+ employees)</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>Healthcare organizations</t>
+  </si>
+  <si>
+    <t>High tech</t>
+  </si>
+  <si>
+    <t>Hospitality</t>
+  </si>
+  <si>
+    <t>Labor</t>
+  </si>
+  <si>
+    <t>Private equity</t>
+  </si>
+  <si>
+    <t>Professional employer organizations</t>
+  </si>
+  <si>
+    <t>Public governments</t>
+  </si>
+  <si>
+    <t>International</t>
+  </si>
+  <si>
+    <t>Pay your bill</t>
+  </si>
+  <si>
+    <t>Manage employee benefits</t>
+  </si>
+  <si>
+    <t>Tools, manuals and forms</t>
+  </si>
+  <si>
+    <t>Contact Aetna</t>
+  </si>
+  <si>
+    <t>Pay your Aetna bill</t>
+  </si>
+  <si>
+    <t>Pay your Innovation Health premiums</t>
+  </si>
+  <si>
+    <t>Resources by region</t>
+  </si>
+  <si>
+    <t>Summary of Benefits</t>
+  </si>
+  <si>
+    <t>Find a doctor or hospital</t>
+  </si>
+  <si>
+    <t>Crisis response support</t>
+  </si>
+  <si>
+    <t>Personalized medicine</t>
+  </si>
+  <si>
+    <t>Precision medicine</t>
   </si>
 </sst>
 </file>
@@ -387,18 +544,486 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{180F5DF7-E53F-4BE8-B03E-62EF8EBCE2BF}">
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="51.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{512CBDDD-41B7-4862-A249-EBCBA3EF1BF8}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FFC4C0E-2855-4180-A7F3-7554313FC21B}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2019CA6-20D1-4CA1-A810-9840DF71F865}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F0A8E5D-AB69-4C8A-B9B2-2D40B5F3EFAD}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A80421B3-EFB6-45C2-AAB6-AA9994DF0523}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1F5D27B-CB73-4F05-AA2C-690E844620A7}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
+    <col min="1" max="1" width="39" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68AA9CFF-3E6C-457E-891C-12AEA6E2A194}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F890DC9-4E61-466B-BB46-54925074261B}">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A5FD9D8-21AA-4EBA-871D-AF67CE56DF34}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F29C8EE3-254E-4222-9ADB-7F12005F5DA2}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2EB20E7-F3E4-4126-B4F5-A3EB30DAB133}">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54B1CF6D-F9F9-415F-9A1B-68980F28171C}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FF95BB6-1BBC-4692-AB2E-CD33C6C6C16F}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>